<commit_message>
Working on the shopping cart, not done
</commit_message>
<xml_diff>
--- a/UpdatedTestCases_Nov24.xlsx
+++ b/UpdatedTestCases_Nov24.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Logging In" sheetId="4" r:id="rId1"/>
-    <sheet name="Registration" sheetId="8" r:id="rId2"/>
-    <sheet name="Purchase A Product" sheetId="1" r:id="rId3"/>
+    <sheet name="Purchase A Product" sheetId="1" r:id="rId1"/>
+    <sheet name="Logging In" sheetId="4" r:id="rId2"/>
+    <sheet name="Registering" sheetId="8" r:id="rId3"/>
     <sheet name="Leave A Review" sheetId="5" r:id="rId4"/>
     <sheet name="Access an Online Course" sheetId="2" r:id="rId5"/>
   </sheets>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="67">
   <si>
     <t>TC ID#</t>
   </si>
@@ -157,6 +157,9 @@
     <t>Password</t>
   </si>
   <si>
+    <t>Message</t>
+  </si>
+  <si>
     <t>Scenario 4 - Empty Field - Username</t>
   </si>
   <si>
@@ -169,9 +172,27 @@
     <t>Scenario 2 - No Username Found</t>
   </si>
   <si>
+    <t>Scenario 3 - Wrong Password - 2 tries left</t>
+  </si>
+  <si>
+    <t>Scenario 4 - Wrong Password - 1 try left</t>
+  </si>
+  <si>
+    <t>Scenario 5 - Wrong Password - 0 tries left</t>
+  </si>
+  <si>
+    <t>Back to Home Page</t>
+  </si>
+  <si>
+    <t>Scenario 6 - Empty Password</t>
+  </si>
+  <si>
     <t>CW7.</t>
   </si>
   <si>
+    <t>Scenario 7 - Empty Username</t>
+  </si>
+  <si>
     <t>View E-Course Catalog</t>
   </si>
   <si>
@@ -203,69 +224,6 @@
   </si>
   <si>
     <t>Error - Online course not found</t>
-  </si>
-  <si>
-    <t>Cannot Login - * Indicator shown</t>
-  </si>
-  <si>
-    <t>CW8.</t>
-  </si>
-  <si>
-    <t>Message - Your login attempt was not successful. Please try again.</t>
-  </si>
-  <si>
-    <t>Message - Password length minimum: 6. Non-alphanumeric characters required: 0.</t>
-  </si>
-  <si>
-    <t>Scenario 4 - Login Credentials not remembered</t>
-  </si>
-  <si>
-    <t>Username and Password are blank</t>
-  </si>
-  <si>
-    <t>Scenario 3 - Wrong Password</t>
-  </si>
-  <si>
-    <t>Scenario 5 - Empty Password</t>
-  </si>
-  <si>
-    <t>Scenario 6 - Empty Username</t>
-  </si>
-  <si>
-    <t>Confirm Password</t>
-  </si>
-  <si>
-    <t>E-mail</t>
-  </si>
-  <si>
-    <t>Security Question</t>
-  </si>
-  <si>
-    <t>Security Answer</t>
-  </si>
-  <si>
-    <t>Scenario 6 - Empty Field - Confirm Password</t>
-  </si>
-  <si>
-    <t>Message - Please enter a different User name</t>
-  </si>
-  <si>
-    <t>Message - * Indicator shown</t>
-  </si>
-  <si>
-    <t>CW9.</t>
-  </si>
-  <si>
-    <t>Scenario 7 - Empty Field - E-Mail</t>
-  </si>
-  <si>
-    <t>Scenario 8 - Empty Field - Security Question</t>
-  </si>
-  <si>
-    <t>Scenario 9 - Empty Field - Security Answer</t>
-  </si>
-  <si>
-    <t>Successful Registration - Redirect to Login Page</t>
   </si>
 </sst>
 </file>
@@ -502,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -556,28 +514,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -852,7 +788,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -860,612 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="6" width="29" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-    </row>
-    <row r="6" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="20"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="F1:F5"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="B1:B5"/>
-    <mergeCell ref="C1:C5"/>
-    <mergeCell ref="D1:D5"/>
-    <mergeCell ref="E1:E5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="10" width="22.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="51" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="I1:I5"/>
-    <mergeCell ref="J1:J5"/>
-    <mergeCell ref="G1:G5"/>
-    <mergeCell ref="H1:H5"/>
-    <mergeCell ref="F1:F5"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="B1:B5"/>
-    <mergeCell ref="C1:C5"/>
-    <mergeCell ref="D1:D5"/>
-    <mergeCell ref="E1:E5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,7 +931,7 @@
         <v>11</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
@@ -1683,12 +1017,408 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F1:F5"/>
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="B1:B5"/>
+    <mergeCell ref="C1:C5"/>
+    <mergeCell ref="D1:D5"/>
+    <mergeCell ref="E1:E5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView zoomScale="133" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F1:F5"/>
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="B1:B5"/>
+    <mergeCell ref="C1:C5"/>
+    <mergeCell ref="D1:D5"/>
+    <mergeCell ref="E1:E5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1775,7 +1505,7 @@
         <v>11</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
@@ -1882,13 +1612,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>2</v>
@@ -1931,7 +1661,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>11</v>
@@ -1943,7 +1673,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1951,7 +1681,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>11</v>
@@ -1963,7 +1693,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
@@ -1971,7 +1701,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>11</v>
@@ -1983,7 +1713,7 @@
         <v>13</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>